<commit_message>
admin panel add setting page
</commit_message>
<xml_diff>
--- a/TEMPS/Databes/Databse.xlsx
+++ b/TEMPS/Databes/Databse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Php\Laravel9-BeautyCenter\TEMPS\Databes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3A3121-12A7-4621-A2D5-52DD2E6F0569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4915572C-B6F3-4ED0-9660-0099F937938D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21765" yWindow="-2430" windowWidth="14115" windowHeight="7875" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
+    <workbookView xWindow="-9990" yWindow="-3000" windowWidth="10140" windowHeight="7875" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="34-Beauty" sheetId="36" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4323" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4331" uniqueCount="371">
   <si>
     <t>Project Main Table</t>
   </si>
@@ -1196,6 +1196,15 @@
   <si>
     <t>tax</t>
   </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
 </sst>
 </file>
 
@@ -1981,6 +1990,62 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>13608</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>176894</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Bağlayıcı: Eğri 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34480E89-5F46-41FC-A8AC-5BB1E2479B13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="251732" y="5694590"/>
+          <a:ext cx="1660072" cy="585107"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14885,10 +14950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9912ED1F-F8BC-4DFC-90B0-559789344068}">
-  <dimension ref="B1:R35"/>
+  <dimension ref="B1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15573,32 +15638,58 @@
       </c>
     </row>
     <row r="30" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="B30" s="54" t="s">
+        <v>370</v>
+      </c>
       <c r="D30" s="54" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="43" t="s">
+        <v>11</v>
+      </c>
       <c r="D31" s="43" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B32" s="43" t="s">
+        <v>13</v>
+      </c>
       <c r="D32" s="43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" s="43" t="s">
+        <v>368</v>
+      </c>
       <c r="D33" s="43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B34" s="43" t="s">
+        <v>369</v>
+      </c>
       <c r="D34" s="43" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B35" s="43" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D35" s="43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B36" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="43" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add contact & about pages and control in admin panel
</commit_message>
<xml_diff>
--- a/TEMPS/Databes/Databse.xlsx
+++ b/TEMPS/Databes/Databse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Php\Laravel9-BeautyCenter\TEMPS\Databes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4915572C-B6F3-4ED0-9660-0099F937938D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105A77EF-2CE0-4541-91BC-F46518C7D8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9990" yWindow="-3000" windowWidth="10140" windowHeight="7875" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
+    <workbookView xWindow="-28920" yWindow="-7005" windowWidth="29040" windowHeight="15990" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="34-Beauty" sheetId="36" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4331" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="372">
   <si>
     <t>Project Main Table</t>
   </si>
@@ -1188,9 +1188,6 @@
     <t>photo_id</t>
   </si>
   <si>
-    <t>social media</t>
-  </si>
-  <si>
     <t>Categories</t>
   </si>
   <si>
@@ -1203,14 +1200,20 @@
     <t>link</t>
   </si>
   <si>
-    <t>pages</t>
+    <t>socialmedia</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>FAQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1266,6 +1269,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1504,7 +1516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1579,6 +1591,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,13 +2009,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
+      <xdr:rowOff>47226</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>176894</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>20012</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2016,8 +2030,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="251732" y="5694590"/>
-          <a:ext cx="1660072" cy="585107"/>
+          <a:off x="248931" y="5558119"/>
+          <a:ext cx="1676080" cy="582706"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -14953,7 +14967,7 @@
   <dimension ref="B1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14985,11 +14999,11 @@
       </c>
     </row>
     <row r="2" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="56" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="56" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1"/>
@@ -14997,15 +15011,15 @@
         <v>3</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="41" t="s">
-        <v>366</v>
+      <c r="H2" s="56" t="s">
+        <v>365</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="56" t="s">
         <v>334</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="56" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="1"/>
@@ -15323,7 +15337,7 @@
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -15609,7 +15623,7 @@
     </row>
     <row r="23" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
-        <v>69</v>
+        <v>371</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="43" t="s">
@@ -15630,19 +15644,24 @@
       <c r="R23" s="15"/>
     </row>
     <row r="24" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="43" t="s">
-        <v>25</v>
+      <c r="B24" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="D24" s="43" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="25" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="43" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="30" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="57" t="s">
         <v>370</v>
       </c>
       <c r="D30" s="54" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -15663,18 +15682,18 @@
     </row>
     <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="43" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="43" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
home page add service detail page
</commit_message>
<xml_diff>
--- a/TEMPS/Databes/Databse.xlsx
+++ b/TEMPS/Databes/Databse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Php\Laravel9-BeautyCenter\TEMPS\Databes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105A77EF-2CE0-4541-91BC-F46518C7D8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D30E75-50E5-42A3-9A5F-CA715BBD3AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-7005" windowWidth="29040" windowHeight="15990" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4345" uniqueCount="373">
   <si>
     <t>Project Main Table</t>
   </si>
@@ -1208,6 +1208,9 @@
   <si>
     <t>FAQ</t>
   </si>
+  <si>
+    <t>hours</t>
+  </si>
 </sst>
 </file>
 
@@ -1588,11 +1591,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1897,13 +1900,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>82922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133353</xdr:rowOff>
+      <xdr:rowOff>178176</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1918,8 +1921,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2524125" y="495299"/>
-          <a:ext cx="3438525" cy="2714629"/>
+          <a:off x="2535331" y="542363"/>
+          <a:ext cx="3442447" cy="2683813"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -14967,7 +14970,7 @@
   <dimension ref="B1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14999,11 +15002,11 @@
       </c>
     </row>
     <row r="2" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="55" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1"/>
@@ -15011,15 +15014,15 @@
         <v>3</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="55" t="s">
         <v>365</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="55" t="s">
         <v>334</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="56" t="s">
+      <c r="L2" s="55" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="1"/>
@@ -15031,7 +15034,7 @@
         <v>9</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="41" t="s">
+      <c r="R2" s="55" t="s">
         <v>10</v>
       </c>
     </row>
@@ -15389,7 +15392,7 @@
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="5" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -15411,8 +15414,8 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="43" t="s">
-        <v>72</v>
+      <c r="J14" s="5" t="s">
+        <v>372</v>
       </c>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
@@ -15436,8 +15439,8 @@
       <c r="G15" s="15"/>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="43" t="s">
-        <v>25</v>
+      <c r="J15" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
@@ -15464,7 +15467,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="43" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
@@ -15491,7 +15494,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="43" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
@@ -15517,7 +15520,9 @@
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+      <c r="J18" s="43" t="s">
+        <v>29</v>
+      </c>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
@@ -15541,6 +15546,9 @@
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
+      <c r="J19" s="43" t="s">
+        <v>35</v>
+      </c>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
@@ -15621,7 +15629,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B23" s="9" t="s">
         <v>371</v>
       </c>
@@ -15634,6 +15642,9 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
+      <c r="J23" s="41" t="s">
+        <v>10</v>
+      </c>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
@@ -15650,18 +15661,47 @@
       <c r="D24" s="43" t="s">
         <v>35</v>
       </c>
+      <c r="J24" s="43" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="43" t="s">
         <v>25</v>
       </c>
+      <c r="J25" s="43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J26" s="43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J27" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J28" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J29" s="43" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="56" t="s">
         <v>370</v>
       </c>
       <c r="D30" s="54" t="s">
         <v>369</v>
+      </c>
+      <c r="J30" s="43" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -15671,6 +15711,9 @@
       <c r="D31" s="43" t="s">
         <v>11</v>
       </c>
+      <c r="J31" s="43" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="43" t="s">
@@ -15679,16 +15722,22 @@
       <c r="D32" s="43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J32" s="43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="43" t="s">
         <v>367</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J33" s="43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="43" t="s">
         <v>368</v>
       </c>
@@ -15696,7 +15745,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="43" t="s">
         <v>29</v>
       </c>
@@ -15704,7 +15753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B36" s="43" t="s">
         <v>35</v>
       </c>
@@ -31052,11 +31101,11 @@
         <v>52</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="55" t="s">
+      <c r="F15" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
       <c r="I15" s="15"/>
       <c r="J15" s="43" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
reviews with jetstream livewire and manage at user and admin panel
</commit_message>
<xml_diff>
--- a/TEMPS/Databes/Databse.xlsx
+++ b/TEMPS/Databes/Databse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Php\Laravel9-BeautyCenter\TEMPS\Databes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D30E75-50E5-42A3-9A5F-CA715BBD3AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B676F296-C6D5-4C62-8CB3-CC1F635D5CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-7005" windowWidth="29040" windowHeight="15990" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="34-Beauty" sheetId="36" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4345" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4334" uniqueCount="374">
   <si>
     <t>Project Main Table</t>
   </si>
@@ -1211,6 +1211,9 @@
   <si>
     <t>hours</t>
   </si>
+  <si>
+    <t>review</t>
+  </si>
 </sst>
 </file>
 
@@ -1269,18 +1272,18 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="0"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1590,12 +1593,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1961,7 +1964,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>176892</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2017,7 +2020,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>20012</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -14967,10 +14970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9912ED1F-F8BC-4DFC-90B0-559789344068}">
-  <dimension ref="B1:R36"/>
+  <dimension ref="B1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15002,27 +15005,27 @@
       </c>
     </row>
     <row r="2" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="54" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="41" t="s">
-        <v>3</v>
+      <c r="F2" s="54" t="s">
+        <v>373</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="54" t="s">
         <v>365</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="54" t="s">
         <v>334</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="54" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="1"/>
@@ -15034,7 +15037,7 @@
         <v>9</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="54" t="s">
         <v>10</v>
       </c>
     </row>
@@ -15629,7 +15632,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>371</v>
       </c>
@@ -15642,9 +15645,6 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
-      <c r="J23" s="41" t="s">
-        <v>10</v>
-      </c>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
@@ -15661,103 +15661,68 @@
       <c r="D24" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="43" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="25" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="43" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J26" s="43" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J27" s="43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J28" s="43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J29" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B30" s="56" t="s">
+    </row>
+    <row r="26" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="B29" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="D30" s="54" t="s">
+      <c r="D29" s="56" t="s">
         <v>369</v>
       </c>
-      <c r="J30" s="43" t="s">
-        <v>32</v>
+    </row>
+    <row r="30" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B30" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B31" s="43" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="J31" s="43" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="43" t="s">
-        <v>13</v>
+        <v>367</v>
       </c>
       <c r="D32" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="43" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" s="43" t="s">
+        <v>368</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B34" s="43" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="43" t="s">
-        <v>367</v>
-      </c>
-      <c r="D33" s="43" t="s">
-        <v>367</v>
-      </c>
-      <c r="J33" s="43" t="s">
+      <c r="D34" s="43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B35" s="43" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B34" s="43" t="s">
-        <v>368</v>
-      </c>
-      <c r="D34" s="43" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B35" s="43" t="s">
-        <v>29</v>
-      </c>
       <c r="D35" s="43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B36" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="43" t="s">
         <v>35</v>
       </c>
     </row>
@@ -31101,11 +31066,11 @@
         <v>52</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="15"/>
       <c r="J15" s="43" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
home page add appointments
</commit_message>
<xml_diff>
--- a/TEMPS/Databes/Databse.xlsx
+++ b/TEMPS/Databes/Databse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Php\Laravel9-BeautyCenter\TEMPS\Databes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B676F296-C6D5-4C62-8CB3-CC1F635D5CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FB6293-5093-4DB3-81E0-95B7E1C954D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
+    <workbookView xWindow="-28920" yWindow="-7005" windowWidth="29040" windowHeight="15990" tabRatio="890" xr2:uid="{6B565FA0-F1C3-422A-B903-82CB9C06F3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="34-Beauty" sheetId="36" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4334" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="374">
   <si>
     <t>Project Main Table</t>
   </si>
@@ -1522,7 +1522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1594,11 +1594,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14972,8 +14973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9912ED1F-F8BC-4DFC-90B0-559789344068}">
   <dimension ref="B1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15029,11 +15030,11 @@
         <v>6</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="58" t="s">
         <v>279</v>
       </c>
       <c r="O2" s="1"/>
-      <c r="P2" s="41" t="s">
+      <c r="P2" s="54" t="s">
         <v>9</v>
       </c>
       <c r="Q2" s="1"/>
@@ -15375,7 +15376,9 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
-      <c r="N12" s="44"/>
+      <c r="N12" s="44" t="s">
+        <v>13</v>
+      </c>
       <c r="O12" s="15"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
@@ -15400,7 +15403,9 @@
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
-      <c r="N13" s="44"/>
+      <c r="N13" s="44" t="s">
+        <v>22</v>
+      </c>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
@@ -15423,7 +15428,9 @@
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="44"/>
+      <c r="N14" s="44" t="s">
+        <v>26</v>
+      </c>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
@@ -15671,10 +15678,10 @@
     <row r="27" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B29" s="57" t="s">
+      <c r="B29" s="56" t="s">
         <v>370</v>
       </c>
-      <c r="D29" s="56" t="s">
+      <c r="D29" s="55" t="s">
         <v>369</v>
       </c>
     </row>
@@ -31066,11 +31073,11 @@
         <v>52</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="55" t="s">
+      <c r="F15" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
       <c r="I15" s="15"/>
       <c r="J15" s="43" t="s">
         <v>25</v>

</xml_diff>